<commit_message>
TestNg ,POM Class , Keyword Driven Framework
</commit_message>
<xml_diff>
--- a/wcsm9automationproject1/src/main/resources/ActiTimeTestData.xlsx
+++ b/wcsm9automationproject1/src/main/resources/ActiTimeTestData.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2430" windowWidth="10710" windowHeight="3960" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="validcreds" sheetId="1" r:id="rId1"/>
     <sheet name="invalidcreds" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Username</t>
   </si>
@@ -24,28 +24,31 @@
     <t>Password</t>
   </si>
   <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
     <t>ad_min</t>
   </si>
   <si>
     <t>mana_ger</t>
   </si>
   <si>
-    <t>manager</t>
-  </si>
-  <si>
-    <t>admin</t>
+    <t>anager</t>
   </si>
   <si>
     <t>123min</t>
   </si>
   <si>
+    <t>ad@min</t>
+  </si>
+  <si>
+    <t>mna@ger</t>
+  </si>
+  <si>
     <t>mana456</t>
-  </si>
-  <si>
-    <t>ad@min</t>
-  </si>
-  <si>
-    <t>mana@ger</t>
   </si>
   <si>
     <t>mana123</t>
@@ -58,7 +61,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,28 +70,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <i/>
       <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,15 +125,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -448,34 +438,33 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" customWidth="1"/>
+    <col min="1" max="1" width="11.08984375" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:2" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -483,83 +472,87 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>12345</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B4" s="3">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
+      <c r="B7" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1"/>
-    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId1" display="mana@ger"/>
+    <hyperlink ref="A6" r:id="rId2"/>
+    <hyperlink ref="B6" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Excution of failed test case and reading the data from xml
</commit_message>
<xml_diff>
--- a/wcsm9automationproject1/src/main/resources/ActiTimeTestData.xlsx
+++ b/wcsm9automationproject1/src/main/resources/ActiTimeTestData.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2430" windowWidth="10710" windowHeight="3960" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2430" windowWidth="10710" windowHeight="3960" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="validcreds" sheetId="1" r:id="rId1"/>
     <sheet name="invalidcreds" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="customer and project creds" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Username</t>
   </si>
@@ -39,22 +39,31 @@
     <t>anager</t>
   </si>
   <si>
-    <t>123min</t>
-  </si>
-  <si>
     <t>ad@min</t>
   </si>
   <si>
     <t>mna@ger</t>
   </si>
   <si>
-    <t>mana456</t>
-  </si>
-  <si>
-    <t>mana123</t>
-  </si>
-  <si>
-    <t>ad123</t>
+    <t>ad</t>
+  </si>
+  <si>
+    <t>mana</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>Customer_Name</t>
+  </si>
+  <si>
+    <t>Project_Name</t>
+  </si>
+  <si>
+    <t>Yes Bank</t>
+  </si>
+  <si>
+    <t>Automate Web Application</t>
   </si>
 </sst>
 </file>
@@ -438,29 +447,29 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" customWidth="1"/>
+    <col min="1" max="1" width="18.26953125" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -472,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B8"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -498,8 +507,8 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
-        <v>12345</v>
+      <c r="A3" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
@@ -509,24 +518,24 @@
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
-        <v>1234</v>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -539,10 +548,10 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -558,12 +567,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.6328125" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>